<commit_message>
db excel updated added full db scripts added new sql file for upgrade scrips
</commit_message>
<xml_diff>
--- a/documents/DB.xlsx
+++ b/documents/DB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="216">
   <si>
     <t>user_role</t>
   </si>
@@ -604,6 +604,66 @@
   </si>
   <si>
     <t>invoice_master</t>
+  </si>
+  <si>
+    <t>store invoices generated for university and third party</t>
+  </si>
+  <si>
+    <t>doc_types are 1. Registartion, 2. Invoice</t>
+  </si>
+  <si>
+    <t>stores all the docs, registration, invoices etc</t>
+  </si>
+  <si>
+    <t>registration_status</t>
+  </si>
+  <si>
+    <t>name of status</t>
+  </si>
+  <si>
+    <t>id from registration_status</t>
+  </si>
+  <si>
+    <t>#27</t>
+  </si>
+  <si>
+    <t>comments about the status</t>
+  </si>
+  <si>
+    <t>#28</t>
+  </si>
+  <si>
+    <t>receipts</t>
+  </si>
+  <si>
+    <t>doc_id</t>
+  </si>
+  <si>
+    <t>doc_amount</t>
+  </si>
+  <si>
+    <t>doc_date</t>
+  </si>
+  <si>
+    <t>narration</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>auto increment number</t>
+  </si>
+  <si>
+    <t>id from document master</t>
+  </si>
+  <si>
+    <t>date of the document</t>
+  </si>
+  <si>
+    <t>document amount</t>
+  </si>
+  <si>
+    <t>receipt amount</t>
   </si>
 </sst>
 </file>
@@ -725,6 +785,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -734,22 +804,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -759,7 +816,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D707"/>
+  <dimension ref="A2:D714"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
-      <selection activeCell="D267" sqref="D267"/>
+    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="K276" sqref="K276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,19 +1139,19 @@
       <c r="A2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1133,21 +1193,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -1225,19 +1285,19 @@
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1293,19 +1353,19 @@
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1349,19 +1409,19 @@
       <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -1495,19 +1555,19 @@
       <c r="A49" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -1659,19 +1719,19 @@
       <c r="A66" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="6"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -1781,19 +1841,19 @@
       <c r="A79" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C79" s="11"/>
-      <c r="D79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="13"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="6"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -1941,19 +2001,19 @@
       <c r="A96" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="12"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="13"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C97" s="5"/>
-      <c r="D97" s="6"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -2001,19 +2061,19 @@
       <c r="A103" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B103" s="10" t="s">
+      <c r="B103" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="13"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="6"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="10"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
@@ -2061,19 +2121,19 @@
       <c r="A110" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B110" s="10" t="s">
+      <c r="B110" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C110" s="11"/>
-      <c r="D110" s="12"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="13"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="6"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="10"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
@@ -2105,19 +2165,19 @@
       <c r="A116" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B116" s="10" t="s">
+      <c r="B116" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C116" s="11"/>
-      <c r="D116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="13"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C117" s="5"/>
-      <c r="D117" s="6"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="10"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
@@ -2249,19 +2309,19 @@
       <c r="A130" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B130" s="10" t="s">
+      <c r="B130" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C130" s="11"/>
-      <c r="D130" s="12"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="13"/>
     </row>
     <row r="131" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
-      <c r="B131" s="15" t="s">
+      <c r="B131" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C131" s="16"/>
-      <c r="D131" s="17"/>
+      <c r="C131" s="15"/>
+      <c r="D131" s="16"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
@@ -2295,19 +2355,19 @@
       <c r="A136" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B136" s="10" t="s">
+      <c r="B136" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C136" s="11"/>
-      <c r="D136" s="12"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="13"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C137" s="5"/>
-      <c r="D137" s="6"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="10"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
@@ -2341,19 +2401,19 @@
       <c r="A142" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="B142" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="9"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="7"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C143" s="5"/>
-      <c r="D143" s="6"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="10"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
@@ -2517,19 +2577,19 @@
       <c r="A160" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B160" s="7" t="s">
+      <c r="B160" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C160" s="8"/>
-      <c r="D160" s="9"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="7"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C161" s="5"/>
-      <c r="D161" s="6"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="10"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
@@ -2629,19 +2689,19 @@
       <c r="A172" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B172" s="7" t="s">
+      <c r="B172" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C172" s="8"/>
-      <c r="D172" s="9"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="7"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
-      <c r="B173" s="4" t="s">
+      <c r="B173" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C173" s="5"/>
-      <c r="D173" s="6"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="10"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
@@ -2685,19 +2745,19 @@
       <c r="A179" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B179" s="7" t="s">
+      <c r="B179" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C179" s="8"/>
-      <c r="D179" s="9"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="7"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
-      <c r="B180" s="4" t="s">
+      <c r="B180" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C180" s="5"/>
-      <c r="D180" s="6"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="10"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
@@ -2745,19 +2805,19 @@
       <c r="A186" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B186" s="7" t="s">
+      <c r="B186" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C186" s="8"/>
-      <c r="D186" s="9"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="7"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C187" s="5"/>
-      <c r="D187" s="6"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="10"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
@@ -2899,19 +2959,17 @@
       <c r="A201" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B201" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C201" s="8"/>
-      <c r="D201" s="9"/>
+      <c r="B201" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C201" s="6"/>
+      <c r="D201" s="7"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3"/>
-      <c r="B202" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C202" s="5"/>
-      <c r="D202" s="6"/>
+      <c r="B202" s="8"/>
+      <c r="C202" s="9"/>
+      <c r="D202" s="10"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
@@ -2928,533 +2986,542 @@
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
       <c r="B204" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
-      <c r="B205" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D205" s="1"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
-      <c r="B206" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="3"/>
-      <c r="B207" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="A207" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C207" s="6"/>
+      <c r="D207" s="7"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
-      <c r="B208" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D208" s="1"/>
+      <c r="B208" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C208" s="9"/>
+      <c r="D208" s="10"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="3"/>
       <c r="B209" s="1" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D209" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="3"/>
       <c r="B210" s="1" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D210" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="3"/>
       <c r="B211" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="D211" s="1"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="3"/>
       <c r="B212" s="1" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="3"/>
       <c r="B213" s="1" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D213" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="3"/>
       <c r="B214" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D214" s="1"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="3"/>
       <c r="B215" s="1" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D215" s="1"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
       <c r="B216" s="1" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D216" s="1"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="3"/>
       <c r="B217" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D217" s="1"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="3"/>
       <c r="B218" s="1" t="s">
-        <v>183</v>
+        <v>21</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3"/>
+      <c r="B219" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D219" s="1"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="3"/>
+      <c r="B220" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D220" s="1"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C221" s="8"/>
-      <c r="D221" s="9"/>
+      <c r="A221" s="3"/>
+      <c r="B221" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="3"/>
-      <c r="B222" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C222" s="5"/>
-      <c r="D222" s="6"/>
+      <c r="B222" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="3"/>
       <c r="B223" s="1" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="3"/>
       <c r="B224" s="1" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="3"/>
       <c r="B225" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>35</v>
+        <v>201</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="3"/>
       <c r="B226" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D226" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="3"/>
-      <c r="B227" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D227" s="1"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
-      <c r="B228" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="3"/>
-      <c r="B229" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D229" s="1"/>
+      <c r="A229" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B229" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C229" s="6"/>
+      <c r="D229" s="7"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="3"/>
-      <c r="B230" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D230" s="1"/>
+      <c r="B230" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C230" s="9"/>
+      <c r="D230" s="10"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="3"/>
       <c r="B231" s="1" t="s">
-        <v>138</v>
+        <v>1</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D231" s="1"/>
+      <c r="D231" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
+      <c r="B232" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="3"/>
+      <c r="B233" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B234" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C234" s="8"/>
-      <c r="D234" s="9"/>
+      <c r="A234" s="3"/>
+      <c r="B234" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D234" s="1"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="3"/>
-      <c r="B235" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C235" s="5"/>
-      <c r="D235" s="6"/>
+      <c r="B235" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D235" s="1"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
       <c r="B236" s="1" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
       <c r="B237" s="1" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D237" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D237" s="1"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
       <c r="B238" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D238" s="1"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
+      <c r="B239" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D239" s="1"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="3" t="s">
+      <c r="A241" s="3"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B241" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C241" s="8"/>
-      <c r="D241" s="9"/>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="3"/>
-      <c r="B242" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C242" s="5"/>
-      <c r="D242" s="6"/>
+      <c r="B242" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C242" s="6"/>
+      <c r="D242" s="7"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
-      <c r="B243" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D243" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B243" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C243" s="9"/>
+      <c r="D243" s="10"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="1" t="s">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="1" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
-      <c r="B246" s="18"/>
-      <c r="C246" s="18"/>
-      <c r="D246" s="18"/>
+      <c r="B246" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D246" s="1"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="3"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B248" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C248" s="8"/>
-      <c r="D248" s="9"/>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="3"/>
-      <c r="B249" s="4"/>
-      <c r="C249" s="5"/>
-      <c r="D249" s="6"/>
+      <c r="B249" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C249" s="6"/>
+      <c r="D249" s="7"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="3"/>
-      <c r="B250" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D250" s="1"/>
+      <c r="B250" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C250" s="9"/>
+      <c r="D250" s="10"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
       <c r="B251" s="1" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D251" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
       <c r="B252" s="1" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D252" s="1"/>
+      <c r="D252" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
       <c r="B253" s="1" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D253" s="1"/>
+      <c r="D253" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="3"/>
-      <c r="B254" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D254" s="1"/>
+      <c r="B254" s="4"/>
+      <c r="C254" s="4"/>
+      <c r="D254" s="4"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="3"/>
-      <c r="B255" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D255" s="1"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="3"/>
-      <c r="B256" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D256" s="1"/>
+      <c r="A256" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C256" s="6"/>
+      <c r="D256" s="7"/>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="3"/>
-      <c r="B257" s="18"/>
-      <c r="C257" s="18"/>
-      <c r="D257" s="18"/>
+      <c r="B257" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C257" s="9"/>
+      <c r="D257" s="10"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="3"/>
+      <c r="B258" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D258" s="1"/>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A259" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B259" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C259" s="8"/>
-      <c r="D259" s="9"/>
+      <c r="A259" s="3"/>
+      <c r="B259" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D259" s="1"/>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="3"/>
-      <c r="B260" s="4"/>
-      <c r="C260" s="5"/>
-      <c r="D260" s="6"/>
+      <c r="B260" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D260" s="1"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="3"/>
       <c r="B261" s="1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>2</v>
@@ -3464,193 +3531,307 @@
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="3"/>
       <c r="B262" s="1" t="s">
-        <v>190</v>
+        <v>58</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D262" s="1"/>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="3"/>
+      <c r="B263" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D263" s="1"/>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="3"/>
+      <c r="B264" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D264" s="1"/>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B265" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C265" s="8"/>
-      <c r="D265" s="9"/>
+      <c r="A265" s="3"/>
+      <c r="B265" s="4"/>
+      <c r="C265" s="4"/>
+      <c r="D265" s="4"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="3"/>
-      <c r="B266" s="4"/>
-      <c r="C266" s="5"/>
-      <c r="D266" s="6"/>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="3"/>
-      <c r="B267" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C267" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D267" s="1"/>
+      <c r="A267" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B267" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C267" s="6"/>
+      <c r="D267" s="7"/>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="3"/>
-      <c r="B268" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C268" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D268" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="B268" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C268" s="9"/>
+      <c r="D268" s="10"/>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="3"/>
       <c r="B269" s="1" t="s">
-        <v>191</v>
+        <v>1</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D269" s="1" t="s">
-        <v>192</v>
-      </c>
+      <c r="D269" s="1"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="3"/>
       <c r="B270" s="1" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="D270" s="1"/>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="3"/>
-      <c r="B271" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D271" s="1"/>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="3"/>
-      <c r="B272" s="1" t="s">
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C273" s="6"/>
+      <c r="D273" s="7"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="3"/>
+      <c r="B274" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C274" s="9"/>
+      <c r="D274" s="10"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="3"/>
+      <c r="B275" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D275" s="1"/>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="3"/>
+      <c r="B276" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="3"/>
+      <c r="B277" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="3"/>
+      <c r="B278" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D278" s="1"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="3"/>
+      <c r="B279" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D279" s="1"/>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="3"/>
+      <c r="B280" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C272" s="1" t="s">
+      <c r="C280" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D272" s="1"/>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="3"/>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="3"/>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="3"/>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="3"/>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="3"/>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="3"/>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" s="3"/>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="3"/>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D280" s="1"/>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="3"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="3"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="3"/>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C283" s="6"/>
+      <c r="D283" s="7"/>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="3"/>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284" s="8"/>
+      <c r="C284" s="9"/>
+      <c r="D284" s="10"/>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="3"/>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="3"/>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="3"/>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="3"/>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D289" s="1"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="3"/>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="3"/>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D291" s="1"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="3"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="3"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="3"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="3"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="3"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="3"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="3"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="3"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="3"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="3"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="3"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="3"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="3"/>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
@@ -4862,14 +5043,69 @@
     <row r="707" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A707" s="3"/>
     </row>
+    <row r="708" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A708" s="3"/>
+    </row>
+    <row r="709" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A709" s="3"/>
+    </row>
+    <row r="710" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A710" s="3"/>
+    </row>
+    <row r="711" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A711" s="3"/>
+    </row>
+    <row r="712" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A712" s="3"/>
+    </row>
+    <row r="713" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A713" s="3"/>
+    </row>
+    <row r="714" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A714" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="B265:D265"/>
-    <mergeCell ref="B266:D266"/>
-    <mergeCell ref="B259:D259"/>
-    <mergeCell ref="B260:D260"/>
-    <mergeCell ref="B248:D248"/>
+  <mergeCells count="56">
+    <mergeCell ref="B201:D201"/>
+    <mergeCell ref="B202:D202"/>
+    <mergeCell ref="B283:D283"/>
+    <mergeCell ref="B284:D284"/>
+    <mergeCell ref="B243:D243"/>
     <mergeCell ref="B249:D249"/>
+    <mergeCell ref="B250:D250"/>
+    <mergeCell ref="B207:D207"/>
+    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="B229:D229"/>
+    <mergeCell ref="B230:D230"/>
+    <mergeCell ref="B242:D242"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="B131:D131"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B137:D137"/>
     <mergeCell ref="B142:D142"/>
     <mergeCell ref="B179:D179"/>
     <mergeCell ref="B180:D180"/>
@@ -4880,42 +5116,12 @@
     <mergeCell ref="B173:D173"/>
     <mergeCell ref="B160:D160"/>
     <mergeCell ref="B172:D172"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B131:D131"/>
-    <mergeCell ref="B136:D136"/>
-    <mergeCell ref="B137:D137"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B235:D235"/>
-    <mergeCell ref="B241:D241"/>
-    <mergeCell ref="B242:D242"/>
-    <mergeCell ref="B201:D201"/>
-    <mergeCell ref="B202:D202"/>
-    <mergeCell ref="B221:D221"/>
-    <mergeCell ref="B222:D222"/>
-    <mergeCell ref="B234:D234"/>
+    <mergeCell ref="B273:D273"/>
+    <mergeCell ref="B274:D274"/>
+    <mergeCell ref="B267:D267"/>
+    <mergeCell ref="B268:D268"/>
+    <mergeCell ref="B256:D256"/>
+    <mergeCell ref="B257:D257"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new excel Forms.xlsx added for form fields
</commit_message>
<xml_diff>
--- a/documents/DB.xlsx
+++ b/documents/DB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="217">
   <si>
     <t>user_role</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>receipt amount</t>
+  </si>
+  <si>
+    <t>pincode</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D714"/>
+  <dimension ref="A2:D715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="K276" sqref="K276"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,163 +2519,163 @@
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="1" t="s">
-        <v>40</v>
+        <v>216</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D153" s="1"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D154" s="1"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D155" s="1"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D157" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
+      <c r="B158" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D158" s="1"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="3"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B161" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C160" s="6"/>
-      <c r="D160" s="7"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="3"/>
-      <c r="B161" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C161" s="9"/>
-      <c r="D161" s="10"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="7"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
-      <c r="B162" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B162" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C162" s="9"/>
+      <c r="D162" s="10"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="1" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="1" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="1" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D165" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D166" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="D166" s="1"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D167" s="1"/>
+      <c r="D167" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D168" s="1"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>2</v>
@@ -2681,416 +2684,416 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
+      <c r="B170" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170" s="1"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
+      <c r="A172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B173" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C172" s="6"/>
-      <c r="D172" s="7"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="3"/>
-      <c r="B173" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C173" s="9"/>
-      <c r="D173" s="10"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="7"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
-      <c r="B174" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B174" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C174" s="9"/>
+      <c r="D174" s="10"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="1" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C176" s="1"/>
-      <c r="D176" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
+      <c r="B177" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
+      <c r="A179" s="3"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B179" s="5" t="s">
+      <c r="B180" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C179" s="6"/>
-      <c r="D179" s="7"/>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="3"/>
-      <c r="B180" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C180" s="9"/>
-      <c r="D180" s="10"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="7"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
-      <c r="B181" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B181" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C181" s="9"/>
+      <c r="D181" s="10"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="1" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="1" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
+      <c r="B184" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="3"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B186" s="5" t="s">
+      <c r="B187" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C186" s="6"/>
-      <c r="D186" s="7"/>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="3"/>
-      <c r="B187" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C187" s="9"/>
-      <c r="D187" s="10"/>
+      <c r="C187" s="6"/>
+      <c r="D187" s="7"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
-      <c r="B188" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C188" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B188" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C188" s="9"/>
+      <c r="D188" s="10"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="1" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="1" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>157</v>
+        <v>2</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="1" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="1" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D193" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="1" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>162</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D194" s="1"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
+      <c r="B199" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="3" t="s">
+      <c r="A201" s="3"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B201" s="5" t="s">
+      <c r="B202" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C201" s="6"/>
-      <c r="D201" s="7"/>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="3"/>
-      <c r="B202" s="8"/>
-      <c r="C202" s="9"/>
-      <c r="D202" s="10"/>
+      <c r="C202" s="6"/>
+      <c r="D202" s="7"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
-      <c r="B203" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B203" s="8"/>
+      <c r="C203" s="9"/>
+      <c r="D203" s="10"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
       <c r="B204" s="1" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>200</v>
+        <v>25</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
+      <c r="B205" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="3" t="s">
+      <c r="A207" s="3"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B207" s="5" t="s">
+      <c r="B208" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C207" s="6"/>
-      <c r="D207" s="7"/>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="3"/>
-      <c r="B208" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C208" s="9"/>
-      <c r="D208" s="10"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="7"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="3"/>
-      <c r="B209" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B209" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C209" s="9"/>
+      <c r="D209" s="10"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="3"/>
       <c r="B210" s="1" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="3"/>
       <c r="B211" s="1" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D211" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="3"/>
       <c r="B212" s="1" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>171</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D212" s="1"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="3"/>
       <c r="B213" s="1" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="3"/>
       <c r="B214" s="1" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D214" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="3"/>
       <c r="B215" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>6</v>
@@ -3100,201 +3103,201 @@
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
       <c r="B216" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D216" s="1"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="3"/>
       <c r="B217" s="1" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D217" s="1"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="3"/>
       <c r="B218" s="1" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>143</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D218" s="1"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3"/>
       <c r="B219" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D219" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="3"/>
       <c r="B220" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D220" s="1"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="3"/>
       <c r="B221" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D221" s="1"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="3"/>
       <c r="B222" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="3"/>
       <c r="B223" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="3"/>
       <c r="B224" s="1" t="s">
-        <v>183</v>
+        <v>120</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="3"/>
       <c r="B225" s="1" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="3"/>
       <c r="B226" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="3"/>
+      <c r="B227" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="3" t="s">
+      <c r="A229" s="3"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B229" s="5" t="s">
+      <c r="B230" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C229" s="6"/>
-      <c r="D229" s="7"/>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="3"/>
-      <c r="B230" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C230" s="9"/>
-      <c r="D230" s="10"/>
+      <c r="C230" s="6"/>
+      <c r="D230" s="7"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="3"/>
-      <c r="B231" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B231" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C231" s="9"/>
+      <c r="D231" s="10"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
       <c r="B232" s="1" t="s">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="3"/>
       <c r="B233" s="1" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="3"/>
       <c r="B234" s="1" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D234" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="3"/>
       <c r="B235" s="1" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>6</v>
@@ -3304,39 +3307,39 @@
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
       <c r="B236" s="1" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D236" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="D236" s="1"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
       <c r="B237" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D237" s="1"/>
+      <c r="D237" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
       <c r="B238" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D238" s="1"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
       <c r="B239" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>2</v>
@@ -3345,183 +3348,183 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
+      <c r="B240" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D240" s="1"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="3" t="s">
+      <c r="A242" s="3"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B242" s="5" t="s">
+      <c r="B243" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C242" s="6"/>
-      <c r="D242" s="7"/>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="3"/>
-      <c r="B243" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C243" s="9"/>
-      <c r="D243" s="10"/>
+      <c r="C243" s="6"/>
+      <c r="D243" s="7"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
-      <c r="B244" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D244" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B244" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C244" s="9"/>
+      <c r="D244" s="10"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="1" t="s">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="1" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D246" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
+      <c r="B247" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D247" s="1"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="3" t="s">
+      <c r="A249" s="3"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B249" s="5" t="s">
+      <c r="B250" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C249" s="6"/>
-      <c r="D249" s="7"/>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="3"/>
-      <c r="B250" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C250" s="9"/>
-      <c r="D250" s="10"/>
+      <c r="C250" s="6"/>
+      <c r="D250" s="7"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
-      <c r="B251" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B251" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C251" s="9"/>
+      <c r="D251" s="10"/>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
       <c r="B252" s="1" t="s">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
       <c r="B253" s="1" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="3"/>
-      <c r="B254" s="4"/>
-      <c r="C254" s="4"/>
-      <c r="D254" s="4"/>
+      <c r="B254" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="3"/>
+      <c r="B255" s="4"/>
+      <c r="C255" s="4"/>
+      <c r="D255" s="4"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="3" t="s">
+      <c r="A256" s="3"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B256" s="5" t="s">
+      <c r="B257" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C256" s="6"/>
-      <c r="D256" s="7"/>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="3"/>
-      <c r="B257" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C257" s="9"/>
-      <c r="D257" s="10"/>
+      <c r="C257" s="6"/>
+      <c r="D257" s="7"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="3"/>
-      <c r="B258" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D258" s="1"/>
+      <c r="B258" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C258" s="9"/>
+      <c r="D258" s="10"/>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="3"/>
       <c r="B259" s="1" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="D259" s="1"/>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="3"/>
       <c r="B260" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="D260" s="1"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="3"/>
       <c r="B261" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>2</v>
@@ -3531,7 +3534,7 @@
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="3"/>
       <c r="B262" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>2</v>
@@ -3541,262 +3544,269 @@
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="3"/>
       <c r="B263" s="1" t="s">
-        <v>186</v>
+        <v>58</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
       <c r="D263" s="1"/>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="3"/>
       <c r="B264" s="1" t="s">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>44</v>
+        <v>187</v>
       </c>
       <c r="D264" s="1"/>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="3"/>
-      <c r="B265" s="4"/>
-      <c r="C265" s="4"/>
-      <c r="D265" s="4"/>
+      <c r="B265" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D265" s="1"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="3"/>
+      <c r="B266" s="4"/>
+      <c r="C266" s="4"/>
+      <c r="D266" s="4"/>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="3" t="s">
+      <c r="A267" s="3"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B267" s="5" t="s">
+      <c r="B268" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C267" s="6"/>
-      <c r="D267" s="7"/>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" s="3"/>
-      <c r="B268" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C268" s="9"/>
-      <c r="D268" s="10"/>
+      <c r="C268" s="6"/>
+      <c r="D268" s="7"/>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="3"/>
-      <c r="B269" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C269" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D269" s="1"/>
+      <c r="B269" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C269" s="9"/>
+      <c r="D269" s="10"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="3"/>
       <c r="B270" s="1" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D270" s="1"/>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="3"/>
+      <c r="B271" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D271" s="1"/>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="3"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="3" t="s">
+      <c r="A273" s="3"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B273" s="5" t="s">
+      <c r="B274" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C273" s="6"/>
-      <c r="D273" s="7"/>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="3"/>
-      <c r="B274" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C274" s="9"/>
-      <c r="D274" s="10"/>
+      <c r="C274" s="6"/>
+      <c r="D274" s="7"/>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="3"/>
-      <c r="B275" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D275" s="1"/>
+      <c r="B275" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C275" s="9"/>
+      <c r="D275" s="10"/>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="3"/>
       <c r="B276" s="1" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D276" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="D276" s="1"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="3"/>
       <c r="B277" s="1" t="s">
-        <v>191</v>
+        <v>97</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="3"/>
       <c r="B278" s="1" t="s">
-        <v>99</v>
+        <v>191</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D278" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="3"/>
       <c r="B279" s="1" t="s">
-        <v>186</v>
+        <v>99</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>187</v>
+        <v>100</v>
       </c>
       <c r="D279" s="1"/>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="3"/>
       <c r="B280" s="1" t="s">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="D280" s="1"/>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="3"/>
+      <c r="B281" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D281" s="1"/>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="3"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="3" t="s">
+      <c r="A283" s="3"/>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B283" s="5" t="s">
+      <c r="B284" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C283" s="6"/>
-      <c r="D283" s="7"/>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="3"/>
-      <c r="B284" s="8"/>
-      <c r="C284" s="9"/>
-      <c r="D284" s="10"/>
+      <c r="C284" s="6"/>
+      <c r="D284" s="7"/>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
-      <c r="B285" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C285" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D285" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B285" s="8"/>
+      <c r="C285" s="9"/>
+      <c r="D285" s="10"/>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="3"/>
       <c r="B286" s="1" t="s">
-        <v>206</v>
+        <v>1</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="3"/>
       <c r="B287" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="3"/>
       <c r="B288" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>187</v>
+        <v>100</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="3"/>
       <c r="B289" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D289" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="3"/>
       <c r="B290" s="1" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>215</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D290" s="1"/>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="3"/>
       <c r="B291" s="1" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D291" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="3"/>
+      <c r="B292" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D292" s="1"/>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="3"/>
@@ -5064,20 +5074,23 @@
     <row r="714" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A714" s="3"/>
     </row>
+    <row r="715" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A715" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="B201:D201"/>
-    <mergeCell ref="B202:D202"/>
-    <mergeCell ref="B283:D283"/>
+    <mergeCell ref="B230:D230"/>
+    <mergeCell ref="B231:D231"/>
+    <mergeCell ref="B243:D243"/>
+    <mergeCell ref="B274:D274"/>
+    <mergeCell ref="B275:D275"/>
+    <mergeCell ref="B268:D268"/>
+    <mergeCell ref="B269:D269"/>
     <mergeCell ref="B284:D284"/>
-    <mergeCell ref="B243:D243"/>
-    <mergeCell ref="B249:D249"/>
+    <mergeCell ref="B285:D285"/>
+    <mergeCell ref="B244:D244"/>
     <mergeCell ref="B250:D250"/>
-    <mergeCell ref="B207:D207"/>
-    <mergeCell ref="B208:D208"/>
-    <mergeCell ref="B229:D229"/>
-    <mergeCell ref="B230:D230"/>
-    <mergeCell ref="B242:D242"/>
+    <mergeCell ref="B251:D251"/>
     <mergeCell ref="B97:D97"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B49:D49"/>
@@ -5106,22 +5119,22 @@
     <mergeCell ref="B131:D131"/>
     <mergeCell ref="B136:D136"/>
     <mergeCell ref="B137:D137"/>
+    <mergeCell ref="B257:D257"/>
+    <mergeCell ref="B258:D258"/>
     <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B179:D179"/>
     <mergeCell ref="B180:D180"/>
-    <mergeCell ref="B186:D186"/>
+    <mergeCell ref="B181:D181"/>
     <mergeCell ref="B187:D187"/>
+    <mergeCell ref="B188:D188"/>
     <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B162:D162"/>
+    <mergeCell ref="B174:D174"/>
     <mergeCell ref="B161:D161"/>
     <mergeCell ref="B173:D173"/>
-    <mergeCell ref="B160:D160"/>
-    <mergeCell ref="B172:D172"/>
-    <mergeCell ref="B273:D273"/>
-    <mergeCell ref="B274:D274"/>
-    <mergeCell ref="B267:D267"/>
-    <mergeCell ref="B268:D268"/>
-    <mergeCell ref="B256:D256"/>
-    <mergeCell ref="B257:D257"/>
+    <mergeCell ref="B202:D202"/>
+    <mergeCell ref="B203:D203"/>
+    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="B209:D209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5132,7 +5145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
new table ref_test_preparation added
</commit_message>
<xml_diff>
--- a/documents/DB.xlsx
+++ b/documents/DB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="229">
   <si>
     <t>user_role</t>
   </si>
@@ -667,6 +667,42 @@
   </si>
   <si>
     <t>pincode</t>
+  </si>
+  <si>
+    <t>#29</t>
+  </si>
+  <si>
+    <t>reg_test_preparation</t>
+  </si>
+  <si>
+    <t>toffel</t>
+  </si>
+  <si>
+    <t>ielts</t>
+  </si>
+  <si>
+    <t>gmat</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>started_coaching</t>
+  </si>
+  <si>
+    <t>looking_for_coaching</t>
+  </si>
+  <si>
+    <t>looking_for_waier</t>
+  </si>
+  <si>
+    <t>regular_or_fasttrack</t>
+  </si>
+  <si>
+    <t>work_experianc</t>
   </si>
 </sst>
 </file>
@@ -810,6 +846,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -818,10 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1124,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D715"/>
+  <dimension ref="A2:D731"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="D167" sqref="D167"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,11 +1186,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1196,21 +1232,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -1288,19 +1324,19 @@
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1356,19 +1392,19 @@
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2320,11 +2356,11 @@
     </row>
     <row r="131" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
-      <c r="B131" s="14" t="s">
+      <c r="B131" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C131" s="15"/>
-      <c r="D131" s="16"/>
+      <c r="C131" s="17"/>
+      <c r="D131" s="18"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
@@ -3482,22 +3518,23 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="3"/>
+      <c r="B256" s="4"/>
+      <c r="C256" s="4"/>
+      <c r="D256" s="4"/>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="C257" s="6"/>
       <c r="D257" s="7"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="3"/>
-      <c r="B258" s="8" t="s">
-        <v>196</v>
-      </c>
+      <c r="B258" s="8"/>
       <c r="C258" s="9"/>
       <c r="D258" s="10"/>
     </row>
@@ -3509,22 +3546,26 @@
       <c r="C259" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D259" s="1"/>
+      <c r="D259" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="3"/>
       <c r="B260" s="1" t="s">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D260" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="3"/>
       <c r="B261" s="1" t="s">
-        <v>97</v>
+        <v>219</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>2</v>
@@ -3534,7 +3575,7 @@
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="3"/>
       <c r="B262" s="1" t="s">
-        <v>82</v>
+        <v>220</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>2</v>
@@ -3544,7 +3585,7 @@
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="3"/>
       <c r="B263" s="1" t="s">
-        <v>58</v>
+        <v>221</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>2</v>
@@ -3554,101 +3595,117 @@
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="3"/>
       <c r="B264" s="1" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
       <c r="D264" s="1"/>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="3"/>
       <c r="B265" s="1" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="D265" s="1"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="3"/>
-      <c r="B266" s="4"/>
-      <c r="C266" s="4"/>
-      <c r="D266" s="4"/>
+      <c r="B266" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D266" s="1"/>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="3"/>
+      <c r="B267" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D267" s="1"/>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B268" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C268" s="6"/>
-      <c r="D268" s="7"/>
+      <c r="A268" s="3"/>
+      <c r="B268" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D268" s="1"/>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="3"/>
-      <c r="B269" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C269" s="9"/>
-      <c r="D269" s="10"/>
+      <c r="B269" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D269" s="1"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="3"/>
       <c r="B270" s="1" t="s">
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D270" s="1"/>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="3"/>
-      <c r="B271" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D271" s="1"/>
+      <c r="B271" s="4"/>
+      <c r="C271" s="4"/>
+      <c r="D271" s="4"/>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="3"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="3"/>
+      <c r="A273" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C273" s="6"/>
+      <c r="D273" s="7"/>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B274" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C274" s="6"/>
-      <c r="D274" s="7"/>
+      <c r="A274" s="3"/>
+      <c r="B274" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C274" s="9"/>
+      <c r="D274" s="10"/>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="3"/>
-      <c r="B275" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C275" s="9"/>
-      <c r="D275" s="10"/>
+      <c r="B275" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D275" s="1"/>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="3"/>
       <c r="B276" s="1" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="D276" s="1"/>
     </row>
@@ -3660,29 +3717,25 @@
       <c r="C277" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D277" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="D277" s="1"/>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="3"/>
       <c r="B278" s="1" t="s">
-        <v>191</v>
+        <v>82</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D278" s="1" t="s">
-        <v>192</v>
-      </c>
+      <c r="D278" s="1"/>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="3"/>
       <c r="B279" s="1" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="D279" s="1"/>
     </row>
@@ -3702,29 +3755,34 @@
         <v>5</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D281" s="1"/>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="3"/>
+      <c r="B282" s="4"/>
+      <c r="C282" s="4"/>
+      <c r="D282" s="4"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="3"/>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C284" s="6"/>
       <c r="D284" s="7"/>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
-      <c r="B285" s="8"/>
+      <c r="B285" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="C285" s="9"/>
       <c r="D285" s="10"/>
     </row>
@@ -3736,92 +3794,105 @@
       <c r="C286" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D286" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="D286" s="1"/>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="3"/>
       <c r="B287" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D287" s="1" t="s">
-        <v>212</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D287" s="1"/>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="3"/>
-      <c r="B288" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D288" s="1" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="3"/>
-      <c r="B289" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D289" s="1" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="3"/>
-      <c r="B290" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D290" s="1"/>
+      <c r="A290" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C290" s="6"/>
+      <c r="D290" s="7"/>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="3"/>
-      <c r="B291" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D291" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="B291" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C291" s="9"/>
+      <c r="D291" s="10"/>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="3"/>
       <c r="B292" s="1" t="s">
-        <v>209</v>
+        <v>1</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="D292" s="1"/>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="3"/>
+      <c r="B293" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="3"/>
+      <c r="B294" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="3"/>
+      <c r="B295" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D295" s="1"/>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="3"/>
+      <c r="B296" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D296" s="1"/>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="3"/>
+      <c r="B297" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D297" s="1"/>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="3"/>
@@ -3830,66 +3901,135 @@
       <c r="A299" s="3"/>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A300" s="3"/>
+      <c r="A300" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B300" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C300" s="6"/>
+      <c r="D300" s="7"/>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="3"/>
+      <c r="B301" s="8"/>
+      <c r="C301" s="9"/>
+      <c r="D301" s="10"/>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="3"/>
+      <c r="B302" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="3"/>
+      <c r="B303" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="3"/>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B304" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="3"/>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B305" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="3"/>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B306" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D306" s="1"/>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="3"/>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B307" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="3"/>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B308" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D308" s="1"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="3"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="3"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="3"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="3"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="3"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="3"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="3"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="3"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="3"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="3"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="3"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="3"/>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
@@ -5077,20 +5217,89 @@
     <row r="715" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A715" s="3"/>
     </row>
+    <row r="716" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A716" s="3"/>
+    </row>
+    <row r="717" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A717" s="3"/>
+    </row>
+    <row r="718" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A718" s="3"/>
+    </row>
+    <row r="719" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A719" s="3"/>
+    </row>
+    <row r="720" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A720" s="3"/>
+    </row>
+    <row r="721" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A721" s="3"/>
+    </row>
+    <row r="722" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A722" s="3"/>
+    </row>
+    <row r="723" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A723" s="3"/>
+    </row>
+    <row r="724" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A724" s="3"/>
+    </row>
+    <row r="725" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A725" s="3"/>
+    </row>
+    <row r="726" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A726" s="3"/>
+    </row>
+    <row r="727" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A727" s="3"/>
+    </row>
+    <row r="728" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A728" s="3"/>
+    </row>
+    <row r="729" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A729" s="3"/>
+    </row>
+    <row r="730" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A730" s="3"/>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A731" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="B230:D230"/>
-    <mergeCell ref="B231:D231"/>
-    <mergeCell ref="B243:D243"/>
-    <mergeCell ref="B274:D274"/>
-    <mergeCell ref="B275:D275"/>
-    <mergeCell ref="B268:D268"/>
-    <mergeCell ref="B269:D269"/>
-    <mergeCell ref="B284:D284"/>
-    <mergeCell ref="B285:D285"/>
-    <mergeCell ref="B244:D244"/>
-    <mergeCell ref="B250:D250"/>
-    <mergeCell ref="B251:D251"/>
+  <mergeCells count="58">
+    <mergeCell ref="B202:D202"/>
+    <mergeCell ref="B203:D203"/>
+    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="B209:D209"/>
+    <mergeCell ref="B257:D257"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B180:D180"/>
+    <mergeCell ref="B181:D181"/>
+    <mergeCell ref="B187:D187"/>
+    <mergeCell ref="B188:D188"/>
+    <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B162:D162"/>
+    <mergeCell ref="B174:D174"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="B131:D131"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B137:D137"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="B97:D97"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B49:D49"/>
@@ -5101,40 +5310,21 @@
     <mergeCell ref="B79:D79"/>
     <mergeCell ref="B80:D80"/>
     <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B131:D131"/>
-    <mergeCell ref="B136:D136"/>
-    <mergeCell ref="B137:D137"/>
-    <mergeCell ref="B257:D257"/>
+    <mergeCell ref="B300:D300"/>
+    <mergeCell ref="B301:D301"/>
+    <mergeCell ref="B244:D244"/>
+    <mergeCell ref="B250:D250"/>
+    <mergeCell ref="B251:D251"/>
+    <mergeCell ref="B273:D273"/>
+    <mergeCell ref="B274:D274"/>
     <mergeCell ref="B258:D258"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B180:D180"/>
-    <mergeCell ref="B181:D181"/>
-    <mergeCell ref="B187:D187"/>
-    <mergeCell ref="B188:D188"/>
-    <mergeCell ref="B143:D143"/>
-    <mergeCell ref="B162:D162"/>
-    <mergeCell ref="B174:D174"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="B202:D202"/>
-    <mergeCell ref="B203:D203"/>
-    <mergeCell ref="B208:D208"/>
-    <mergeCell ref="B209:D209"/>
+    <mergeCell ref="B230:D230"/>
+    <mergeCell ref="B231:D231"/>
+    <mergeCell ref="B243:D243"/>
+    <mergeCell ref="B290:D290"/>
+    <mergeCell ref="B291:D291"/>
+    <mergeCell ref="B284:D284"/>
+    <mergeCell ref="B285:D285"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>